<commit_message>
DataStructure once more modified. PERIOD in v1.0.3 transformed into DESCRIPTION
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy(Data-Structures)_V1.0.3.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy(Data-Structures)_V1.0.3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD-Steps\ESPD\dist\cl\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="22" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -2153,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15050,7 +15050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>